<commit_message>
Allemployees page arrangements client & Server side
</commit_message>
<xml_diff>
--- a/backend/employeesUpdated.xlsx
+++ b/backend/employeesUpdated.xlsx
@@ -19,7 +19,6 @@
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
-    <style:font-face style:name="Liberation Serif" svg:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans Arabic" svg:font-family="'Noto Sans Arabic'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans Devanagari" svg:font-family="'Noto Sans Devanagari'" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -38,73 +37,73 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="2.752in"/>
     </style:style>
     <style:style style:name="co5" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.6638in"/>
+    </style:style>
+    <style:style style:name="co6" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.3602in"/>
     </style:style>
-    <style:style style:name="co6" style:family="table-column">
+    <style:style style:name="co7" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.3319in"/>
     </style:style>
-    <style:style style:name="co7" style:family="table-column">
+    <style:style style:name="co8" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.1756in"/>
     </style:style>
-    <style:style style:name="co8" style:family="table-column">
+    <style:style style:name="co9" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.6134in"/>
     </style:style>
-    <style:style style:name="co9" style:family="table-column">
+    <style:style style:name="co10" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="4.0252in"/>
     </style:style>
-    <style:style style:name="co10" style:family="table-column">
+    <style:style style:name="co11" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.5846in"/>
     </style:style>
-    <style:style style:name="co11" style:family="table-column">
+    <style:style style:name="co12" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.9244in"/>
     </style:style>
-    <style:style style:name="co12" style:family="table-column">
+    <style:style style:name="co13" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.3709in"/>
     </style:style>
-    <style:style style:name="co13" style:family="table-column">
+    <style:style style:name="co14" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.9047in"/>
     </style:style>
-    <style:style style:name="co14" style:family="table-column">
+    <style:style style:name="co15" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="2.878in"/>
     </style:style>
-    <style:style style:name="co15" style:family="table-column">
+    <style:style style:name="co16" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.2634in"/>
     </style:style>
-    <style:style style:name="co16" style:family="table-column">
+    <style:style style:name="co17" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.1472in"/>
     </style:style>
-    <style:style style:name="co17" style:family="table-column">
+    <style:style style:name="co18" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.9134in"/>
     </style:style>
-    <style:style style:name="co18" style:family="table-column">
+    <style:style style:name="co19" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.1374in"/>
     </style:style>
-    <style:style style:name="co19" style:family="table-column">
+    <style:style style:name="co20" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.7583in"/>
     </style:style>
-    <style:style style:name="co20" style:family="table-column">
+    <style:style style:name="co21" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.4098in"/>
     </style:style>
-    <style:style style:name="co21" style:family="table-column">
+    <style:style style:name="co22" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.7898in"/>
     </style:style>
-    <style:style style:name="co22" style:family="table-column">
+    <style:style style:name="co23" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.3807in"/>
     </style:style>
-    <style:style style:name="co23" style:family="table-column">
+    <style:style style:name="co24" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.972in"/>
     </style:style>
-    <style:style style:name="co24" style:family="table-column">
+    <style:style style:name="co25" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="3.6945in"/>
     </style:style>
-    <style:style style:name="co25" style:family="table-column">
+    <style:style style:name="co26" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="3.6752in"/>
     </style:style>
-    <style:style style:name="co26" style:family="table-column">
+    <style:style style:name="co27" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.752in"/>
-    </style:style>
-    <style:style style:name="co27" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="0.889in"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
       <style:table-row-properties style:row-height="0.478in" fo:break-before="auto" style:use-optimal-row-height="false"/>
@@ -113,12 +112,15 @@
       <style:table-row-properties style:row-height="0.8291in" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro3" style:family="table-row">
-      <style:table-row-properties style:row-height="1.6783in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="1.7854in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro4" style:family="table-row">
       <style:table-row-properties style:row-height="1.8862in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro5" style:family="table-row">
+      <style:table-row-properties style:row-height="1.6783in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro6" style:family="table-row">
       <style:table-row-properties style:row-height="0.1917in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="PageStyle_5f_גיליון1">
@@ -127,6 +129,13 @@
     <number:text-style style:name="N100">
       <number:text-content/>
     </number:text-style>
+    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+      <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
+      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
+        <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
+      </style:text-properties>
+    </style:style>
     <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
@@ -134,14 +143,7 @@
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
-      <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
-      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
-        <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
-      </style:text-properties>
-    </style:style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:background-color="#dae3f3" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto">
         <loext:background-complex-color loext:theme-type="accent1" loext:color-type="theme">
           <loext:transformation loext:type="lummod" loext:value="2001"/>
@@ -157,7 +159,12 @@
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
     </style:style>
-    <style:style style:name="ce21" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
+    <style:style style:name="ce10" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
+      <style:text-properties style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" fo:language="en" fo:country="US" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="DejaVu Sans" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Noto Sans Arabic" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="ce13" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
       <style:table-cell-properties fo:background-color="#dae3f3" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto">
         <loext:background-complex-color loext:theme-type="accent1" loext:color-type="theme">
           <loext:transformation loext:type="lummod" loext:value="2001"/>
@@ -169,14 +176,14 @@
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce22" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
+    <style:style style:name="ce18" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N135">
+    <style:style style:name="ce19" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N135">
       <style:table-cell-properties fo:background-color="#dae3f3" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto">
         <loext:background-complex-color loext:theme-type="accent1" loext:color-type="theme">
           <loext:transformation loext:type="lummod" loext:value="2001"/>
@@ -188,14 +195,14 @@
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N135">
+    <style:style style:name="ce20" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N135">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce8" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N135">
+    <style:style style:name="ce23" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N135">
       <style:table-cell-properties fo:background-color="#dae3f3" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto">
         <loext:background-complex-color loext:theme-type="accent1" loext:color-type="theme">
           <loext:transformation loext:type="lummod" loext:value="2001"/>
@@ -208,7 +215,7 @@
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
     </style:style>
-    <style:style style:name="ce10" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce25" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:background-color="#dae3f3" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto">
         <loext:background-complex-color loext:theme-type="accent1" loext:color-type="theme">
           <loext:transformation loext:type="lummod" loext:value="2001"/>
@@ -224,25 +231,25 @@
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
     </style:style>
-    <style:style style:name="ce29" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce27" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
     </style:style>
-    <style:style style:name="ce30" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce28" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce14" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce29" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:border-bottom="none" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border-left="0.74pt solid #000000" style:direction="ltr" fo:border-right="0.74pt solid #000000" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" fo:border-top="none" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce30" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:border-bottom="none" fo:background-color="#dae3f3" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border-left="0.74pt solid #000000" style:direction="ltr" fo:border-right="0.74pt solid #000000" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" fo:border-top="none" style:vertical-align="middle" loext:vertical-justify="auto">
         <loext:background-complex-color loext:theme-type="accent1" loext:color-type="theme">
           <loext:transformation loext:type="lummod" loext:value="2001"/>
@@ -254,7 +261,7 @@
         <loext:char-complex-color loext:theme-type="dark1" loext:color-type="theme"/>
       </style:text-properties>
     </style:style>
-    <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
+    <style:style style:name="ce31" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="top" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal">
@@ -277,165 +284,170 @@
         <table:table-column table:style-name="co2" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co4" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co5" table:number-columns-repeated="2" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co5" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co6" table:number-columns-repeated="2" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co7" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co8" table:number-columns-repeated="2" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co9" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co8" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co9" table:number-columns-repeated="2" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co10" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co11" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co12" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co13" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co10" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co14" table:default-cell-style-name="ce11"/>
-        <table:table-column table:style-name="co7" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co15" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co14" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co11" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co15" table:default-cell-style-name="ce11"/>
+        <table:table-column table:style-name="co8" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co16" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co17" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co13" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co18" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co14" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co19" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co20" table:number-columns-repeated="2" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co21" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co20" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co21" table:number-columns-repeated="2" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co22" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co23" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co24" table:default-cell-style-name="ce17"/>
+        <table:table-column table:style-name="co24" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co25" table:default-cell-style-name="ce17"/>
-        <table:table-column table:style-name="co26" table:number-columns-repeated="16352" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co26" table:default-cell-style-name="ce17"/>
+        <table:table-column table:style-name="co27" table:number-columns-repeated="16352"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>fullName</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>employeeOfManagerId</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>id</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>role</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
-            <text:p>DateOfBirth</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+            <text:p>team</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+            <text:p>DataOfBirth</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>PlaceOfResidence</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>FamilyStatus</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>NumOfChildren</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Seniority</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Anniversary</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="6" table:number-rows-spanned="1">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="6" table:number-rows-spanned="1">
             <text:p>LatestActivity</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="5" table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:covered-table-cell table:number-columns-repeated="5" table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>InterestingFact</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
             <text:p>ClosestPersonalEvent</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
+          <table:covered-table-cell table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
             <text:p>singers</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
+          <table:covered-table-cell table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
             <text:p>FoodAndDrinks</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce30"/>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
             <text:p>Restaurants</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce30"/>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
+          <table:covered-table-cell table:style-name="ce28"/>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
             <text:p>Hobbies</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce16" office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce31" office:value-type="string" calcext:value-type="string">
             <text:p>TopInsights</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce16" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce31" office:value-type="string" calcext:value-type="string">
             <text:p>LatestInfo</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:covered-table-cell table:number-columns-repeated="10" table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="6" table:number-rows-spanned="1">
+          <table:covered-table-cell table:number-columns-repeated="11" table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="6" table:number-rows-spanned="1">
             <text:p>LatestActivity</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="6" table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Event</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Date</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
             <text:p>singers</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
+          <table:covered-table-cell table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
             <text:p>FoodAndDrinks</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce30"/>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="2" table:number-rows-spanned="1">
             <text:p>Restaurants</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce30"/>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
+          <table:covered-table-cell table:style-name="ce28"/>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
             <text:p>Hobbies</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce4"/>
-          <table:table-cell table:style-name="ce16" office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce1"/>
+          <table:table-cell table:style-name="ce31" office:value-type="string" calcext:value-type="string">
             <text:p>TopInsights</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce16" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce31" office:value-type="string" calcext:value-type="string">
             <text:p>LatestInfo</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Brad Jones</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="1" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>UX/UI Designer</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cf</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>20/04/1990</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Tel Aviv</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>In a Relationship</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="3" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="3" calcext:value-type="float">
             <text:p>3</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>4/2</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "29/03/2024",</text:p>
             <text:p>    "Activity1": "Birthday gift",</text:p>
@@ -445,58 +457,58 @@
             <text:p>    "Activity3": "Promotion"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2024-01-10" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2024-01-10" calcext:value-type="date">
             <text:p>1/10/2024</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Development plan</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-08-21" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-08-21" calcext:value-type="date">
             <text:p>8/21/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Compensation </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Will never miss a game of liverpool</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "12/7", "event": "Spous's birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>12/7</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Adele"}, {"singer": "Ed Sheeran"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Shlomo Artzi</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Do not drink", "Food1": "Ice cream", "Food2": "Sushi"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Ice cream</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Sushi</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Moon sushi", "Restaurant2": "Minna tomei"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Minna tomei</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Soccer", "Hobby2": "Baking", "Hobby3": "Cuban cigars"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Baking</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Cuban cigars</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -513,40 +525,42 @@
             <text:p>  "Info3": "Loves to bake and cook"</text:p>
             <text:p>}</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>John Perkins</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="2" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="2" calcext:value-type="float">
             <text:p>2</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Chief Scientist</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cc</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>12/12/1985</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Jerusalem</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
-            <text:p>Divorced</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="4" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>Divorce</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="4" calcext:value-type="float">
             <text:p>4</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="12" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="12" calcext:value-type="float">
             <text:p>12</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>12/1</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "10/01/2024",</text:p>
             <text:p>    "Activity1": "Personal interview",</text:p>
@@ -556,61 +570,61 @@
             <text:p>    "Activity3": "Compensation"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Assignment feedback</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-12-28" calcext:value-type="date">
             <text:p>12/28/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-09-03" calcext:value-type="date">
             <text:p>9/3/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Birthday gift</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Driving a motorcycle for 20 years</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "1/8", "event": "Child's birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>1/8</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Amir Dadon"},{"singer": "Queen"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{singer: 'Queen'}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"Drink": "Beer", "Food1": "Italian", "Food2": "Meet"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Italian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Meet</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Moshbutz", "Restaurant2": "Hudson"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Hudson </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Drinking beer", "Hobby2": "Playing the piano", "Hobby3": "Swimming"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Playing the piano</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Swimming</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -627,40 +641,42 @@
             <text:p>    "Info3": "Driving a motorcycle for 20 years"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Lisa Robinson</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="3" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="3" calcext:value-type="float">
             <text:p>3</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Data Analyst</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1d0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>09/01/2000</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Kfar Saba</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Single</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="1" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>29/10</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
             <text:p> {</text:p>
             <text:p>    "date1": "03/03/2024",</text:p>
             <text:p>    "Activity1": "Development plan",</text:p>
@@ -670,64 +686,64 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Compensation </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-12-15" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-12-15" calcext:value-type="date">
             <text:p>12/15/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Promotion</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-07-28" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-07-28" calcext:value-type="date">
             <text:p>7/28/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Can drink a good beer at any hour</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s text:c="2"/>
               {"date": "29/10", "event": "Anniversary"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>29/10</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Idan Raichel"}, {"singer": "Shlomo Artzi"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               Red Band
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Wine", "Food1": "Vegetarian", "Food2": "Sushi"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Vegetarian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Sushi</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Moon sushi", "Restaurant2": "Machneyuda"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Machneyuda</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Cooking", "Hobby2": "Salsa dancing", "Hobby3": "Basketball"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Salsa dancing</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Basketball</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -744,40 +760,42 @@
             <text:p>    "Info3": "Can drink a good beer at any hour"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Tom Hill</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="4" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="4" calcext:value-type="float">
             <text:p>4</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Data Analyst</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1d0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>27/09/1998</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Pardes Hanna</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Single</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="4" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="4" calcext:value-type="float">
             <text:p>4</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>13/5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
             <text:p> {</text:p>
             <text:p>    "date1": "08/03/2024",</text:p>
             <text:p>    "Activity1": "Professional training",</text:p>
@@ -787,61 +805,61 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Birthday gift</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-11-05" calcext:value-type="date">
             <text:p>11/5/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-10-16" calcext:value-type="date">
             <text:p>10/16/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Development plan</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>One of the biggests fans of Ed Sheeran</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "13/5", "event": "Anniversary"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>13/5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Idan Raichel"}, {"singer": "red band"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Noa Kirel</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"Drink": "Cocktails", "Food1": "Italian", "Food2": "Thai"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Italian </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Thai</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Tzafririm", "Restaurant2": "Cafe italia"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Cafe italia</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Baking", "Hobby2": "Painting", "Hobby3": "Movies"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Painting</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Movies</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -858,40 +876,42 @@
             <text:p>    "Info3": "One of the biggest fans of Ed Sheeran"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>David Lee</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="5" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="5" calcext:value-type="float">
             <text:p>5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Product Manager</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cd</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>08/07/2003</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Givatayim</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>In a Relationship</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="1" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>4/2</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "10/01/2024",</text:p>
             <text:p>    "Activity1": "Development plan",</text:p>
@@ -901,67 +921,67 @@
             <text:p>    "Activity3": "Birthday gift"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-10-19" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-10-19" calcext:value-type="date">
             <text:p>10/19/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Compensation </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-06-01" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-06-01" calcext:value-type="date">
             <text:p>6/1/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Promotion</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Was a proffesional tennis player</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s text:c="2"/>
               {"date": "8/7", "event": "Birthday"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>8/7</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "miri mesika"}, {"singer": "Shlomo Artzi"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               Red Band
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"Drink": "Whiskey", "Food1": "Ice cream", "Food2": "Italian"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Ice cream</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Italian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Alena", "Restaurant2": "Yafo Tel Aviv"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Yafo Tel Aviv</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Reading books", "Hobby2": "Fishing", "Hobby3": "Photography"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Fishing</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Photography</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -978,40 +998,42 @@
             <text:p>    "Info3": "Has birthday in 3 weeks"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Nicole Miller</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="6" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="6" calcext:value-type="float">
             <text:p>6</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>UX/UI Designer</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cf</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>17/05/1997</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Shoham</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>In a Relationship</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="5" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="5" calcext:value-type="float">
             <text:p>5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>24/6</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "28/12/2023",</text:p>
             <text:p>    "Activity1": "Personal interview",</text:p>
@@ -1021,61 +1043,61 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Promotion</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-11-24" calcext:value-type="date">
             <text:p>11/24/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Compensation </text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-08-13" calcext:value-type="date">
             <text:p>8/13/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Allergic to gluten and eggs </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "17/5", "event": "Birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>17/5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Beatles"}, {"singer": "noa kirel"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Shlomo Artzi</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Wine", "Food1": "Mexican", "Food2": "Veagan"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Mexican </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Veagan</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"Restaurant1": "Anastasia", "Restaurant2": "HaTaco"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>HaTaco</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Yoga", "Hobby2": "Movies", "Hobby3": "Camping"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce14" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce29" office:value-type="string" calcext:value-type="string">
             <text:p>Movies</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Camping</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1092,40 +1114,42 @@
             <text:p>    "Info3": "Allergic to gluten and eggs"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Emma Carter</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="7" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="7" calcext:value-type="float">
             <text:p>7</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Project Manager</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cd</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>10/10/1988</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Tel Aviv</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>married</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="3" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="3" calcext:value-type="float">
             <text:p>3</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="7" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="7" calcext:value-type="float">
             <text:p>7</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>1/9</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "19/10/2023",</text:p>
             <text:p>    "Activity1": "Compensation",</text:p>
@@ -1135,58 +1159,58 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Development plan</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-12-29" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-12-29" calcext:value-type="date">
             <text:p>12/29/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-07-19" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-07-19" calcext:value-type="date">
             <text:p>7/19/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Assignment feedback</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce25" office:value-type="string" calcext:value-type="string">
             <text:p>Visited more then 50 countries before she was 35</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "23/6", "event": "Child's birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>23/6</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Taylor Swift"}, {"singer": "Miri Mesika"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Miri Mesika</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Cocktails", "Food1": "Mediterranean", "Food2": "Pizza"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Mediterranean</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Pizza</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce25" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Triger meat &amp; wine", "Restaurant2": "La Piedra"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>La Piedra</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Camping", "Hobby2": "Building puzzles", "Hobby3": "Soccer"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Building puzzels</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Soccer</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1203,40 +1227,42 @@
             <text:p>    "Info3": "Visited more than 50 countries before she was 35"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Sofia Garcia</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="8" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="8" calcext:value-type="float">
             <text:p>8</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Business Development Manager</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cc</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>06/11/2000</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Bareket</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Single</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="3" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="3" calcext:value-type="float">
             <text:p>3</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>28/3</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
             <text:p> {</text:p>
             <text:p>    "date1": "18/10/2023",</text:p>
             <text:p>    "Activity1": "Development plan",</text:p>
@@ -1246,61 +1272,61 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Proffesional training</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-10-18" calcext:value-type="date">
             <text:p>10/18/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Development plan</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-06-05" calcext:value-type="date">
             <text:p>6/5/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Has a dream to be a famous singer</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "6/11", "event": "Birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>6/11</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "eyal golan"}, {"singer": "ed sheeran"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Ed Sheeran</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s text:c="2"/>
               {"Drink": "Whiskey", "Food1": "Indian", "Food2": "Meet"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Indian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Meet</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Tandoori", "Restaurant2": "Yafo Tel Aviv"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Yafo Tel Aviv</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Swimming", "Hobby2": "Reading books", "Hobby3": "Dogs"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Reading books</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Dogs</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1317,40 +1343,42 @@
             <text:p>    "Info3": "Has a dream to be a famous singer"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Mark Morris</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="9" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="9" calcext:value-type="float">
             <text:p>9</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Research Engineer</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1cc</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>13/03/1994</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Neve Yarak</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>In a Relationship</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="9" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="9" calcext:value-type="float">
             <text:p>9</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>17/7</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "12/09/2023",</text:p>
             <text:p>    "Activity1": "Professional training",</text:p>
@@ -1360,70 +1388,70 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2024-01-02" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2024-01-02" calcext:value-type="date">
             <text:p>1/2/2024</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Birthday gift</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-09-27" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-09-27" calcext:value-type="date">
             <text:p>9/27/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Compensation </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Speaks 5 languages </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"date": "17/7", "event": "Anniversary"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>17/7</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Idan Raichel"}, {"singer": "red band"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Idan Raichel</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Beer", "Food1": "Indian", "Food2": "Asian"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Indian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Asian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"Restaurant1": "Tandoori", "Restaurant2": "Taizu"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Taizu</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s text:c="2"/>
               {"Hobby1": "Horse riding", "Hobby2": "Basketball", "Hobby3": "Drinking beer"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s text:c="2"/>
               Basketball
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Drinking beer</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1440,40 +1468,42 @@
             <text:p>    "Info3": "Will celebrate his anniversary next month"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Josh Williams</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="10" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="10" calcext:value-type="float">
             <text:p>10</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Data Analyst</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1d0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>05/08/1999</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Tel Aviv</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>married</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="1" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="2" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="2" calcext:value-type="float">
             <text:p>2</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>9/4</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "19/07/2023",</text:p>
             <text:p>    "Activity1": "Assignment feedback",</text:p>
@@ -1483,63 +1513,63 @@
             <text:p>    "Activity3": "Compensation"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Proffesional training</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-11-04" calcext:value-type="date">
             <text:p>11/4/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-08-25" calcext:value-type="date">
             <text:p>8/25/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Assignment feedback</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Has a collection of over 50 shoes</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "5/8", "event": "Birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>5/8</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "miri mesika"}, {"singer": "Shlomo Artzi"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Noa Kirel</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:s/>
               {"Drink": "Beer", "Food1": "Vegetarian", "Food2": "Pizza"}
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Vegetarian</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Pizza</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "HaPizza", "Restaurant2": "Anastasia"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:a xlink:href="https://www.secrettelaviv.com/best/anastasia/" xlink:type="simple">Anastasia</text:a>
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Hiking", "Hobby2": "Yoga", "Hobby3": "Camping"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Yoga</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Camping</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1556,40 +1586,42 @@
             <text:p>    "Info3": "Has a collection of over 50 shoes"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Justin Smith</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="11" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="11" calcext:value-type="float">
             <text:p>11</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Research Engineer</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1ce</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>24/12/1995</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Hod Hasharon</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>married</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="2" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="2" calcext:value-type="float">
             <text:p>2</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="6" calcext:value-type="float">
+          <table:table-cell table:style-name="ce5" office:value-type="float" office:value="6" calcext:value-type="float">
             <text:p>6</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>11/8</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "16/10/2023",</text:p>
             <text:p>    "Activity1": "Development plan",</text:p>
@@ -1599,58 +1631,58 @@
             <text:p>    "Activity3": "Personal interview"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Compensation </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-09-12" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-09-12" calcext:value-type="date">
             <text:p>9/12/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Proffesional training</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce8" office:value-type="date" office:date-value="2023-06-04" calcext:value-type="date">
+          <table:table-cell table:style-name="ce23" office:value-type="date" office:date-value="2023-06-04" calcext:value-type="date">
             <text:p>6/4/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Won 5 photography contests</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "9/6", "event": "Spous's birthday"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>9/6</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "omer adam"}, {"singer": "Shlomo Artzi"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Amir Dadon</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Do not drink", "Food1": "Sushi", "Food2": "Meet"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Sushi</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Meet</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "Moon sushi", "Restaurant2": "Makom Shel Basar"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Makom Shel Basar</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Photography", "Hobby2": "Salsa dancing", "Hobby3": "Movies"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Zalsa dancing</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string">
             <text:p>Movies</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1667,40 +1699,42 @@
             <text:p>    "Info3": "His spouse's birthday is one week away"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro5">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Selena Ramos</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="12" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="12" calcext:value-type="float">
             <text:p>12</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Data Analyst</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>66914f4d4e9e6e8d3811a1d0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>01/10/1992</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Beer Sheva</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>married</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="2" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="2" calcext:value-type="float">
             <text:p>2</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="float" office:value="10" calcext:value-type="float">
+          <table:table-cell table:style-name="ce4" office:value-type="float" office:value="10" calcext:value-type="float">
             <text:p>10</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>21/5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
             <text:p>{</text:p>
             <text:p>    "date1": "25/08/2023",</text:p>
             <text:p>    "Activity1": "Assignment feedback",</text:p>
@@ -1710,58 +1744,58 @@
             <text:p>    "Activity3": "Development plan"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Personal interview</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-10-08" calcext:value-type="date">
             <text:p>10/8/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Birthday gift</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="date" office:date-value="2023-07-20" calcext:value-type="date">
             <text:p>7/20/2023</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Development plan</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Has 2 dogs and 4 cats</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"date": "21/5", "event": "Anniversary"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce22" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>21/5</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"singer": "Moshik afia"}, {"singer": "eminem"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Beatles</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Drink": "Wine", "Food1": "Mediterranean", "Food2": "Pizza"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Mediterranean </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Pizza</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Restaurant1": "HaPizza", "Restaurant2": "Triger meat &amp; wine"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce30" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Triger meat &amp; wine</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>{"Hobby1": "Airplane models", "Hobby2": "Drinking wine", "Hobby3": "Dogs"}</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Drinking wine</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Dogs</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1778,22 +1812,21 @@
             <text:p>    "Info3": "Considering taking a long vacation"</text:p>
             <text:p>  }</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="16352"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5" table:number-rows-repeated="6">
-          <table:table-cell table:number-columns-repeated="16383"/>
+        <table:table-row table:style-name="ro6" table:number-rows-repeated="6">
+          <table:table-cell table:number-columns-repeated="32"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5">
-          <table:table-cell table:number-columns-repeated="19"/>
-          <table:table-cell table:style-name="ce29" table:number-columns-spanned="10" table:number-rows-spanned="1"/>
-          <table:covered-table-cell table:number-columns-repeated="9" table:style-name="ce29"/>
-          <table:table-cell table:number-columns-repeated="16354"/>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell table:number-columns-repeated="20"/>
+          <table:table-cell table:style-name="ce27" table:number-columns-spanned="10" table:number-rows-spanned="1"/>
+          <table:covered-table-cell table:number-columns-repeated="9" table:style-name="ce27"/>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5" table:number-rows-repeated="1048554">
-          <table:table-cell table:number-columns-repeated="16383"/>
+        <table:table-row table:style-name="ro6" table:number-rows-repeated="1048554">
+          <table:table-cell table:number-columns-repeated="32"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5">
-          <table:table-cell table:number-columns-repeated="16383"/>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell table:number-columns-repeated="32"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -1808,11 +1841,11 @@
     <meta:creation-date>2024-04-10T19:53:20</meta:creation-date>
     <meta:initial-creator>N</meta:initial-creator>
     <dc:language>en-US</dc:language>
-    <dc:date>2024-07-17T12:07:22.963015271</dc:date>
-    <meta:editing-cycles>9</meta:editing-cycles>
-    <meta:editing-duration>PT6H3M12S</meta:editing-duration>
-    <meta:generator>LibreOffice/24.2.4.2$Linux_X86_64 LibreOffice_project/420$Build-2</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="400" meta:object-count="0"/>
+    <dc:date>2024-07-17T21:36:42.271557135</dc:date>
+    <meta:editing-cycles>14</meta:editing-cycles>
+    <meta:editing-duration>PT6H51M45S</meta:editing-duration>
+    <meta:generator>LibreOffice/7.6.7.2$Linux_X86_64 LibreOffice_project/60$Build-2</meta:generator>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="413" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">15.0000</meta:user-defined>
   </office:meta>
 </office:document-meta>
@@ -1824,15 +1857,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">126825</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">58942</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">133592</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">59214</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="גיליון1">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -1849,7 +1882,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">גיליון1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1783</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">2419</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">65</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -1908,9 +1941,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">MFC-1910W-series</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">wAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMArAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmYMAFBSSU5URVJfTkFNRQ8AR2VuZXJpYyBQcmludGVyCwBEUklWRVJfTkFNRQcAU0dFTlBSVA==</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">7QH+/01GQy0xOTEwVy1zZXJpZXMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpNRkMtMTkxMFctc2VyaWVzAAAAAAAAAAAAAAAWAAMAxgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9TUZDLTE5MTBXLXNlcmllcwpvcmllbnRhdGlvbj1Qb3J0cmFpdApjb3BpZXM9MQpjb2xsYXRlPWZhbHNlCm1hcmdpbmFkanVzdG1lbnQ9MCwwLCcwLDAKY29sb3JkZXB0aD0yNApwc2xldmVsPTAKcGRmZGV2aWNlPTEKY29sb3JkZXZpY2U9MApQUERDb250ZXh0RGF0YQpQYWdlU2l6ZTpBNABJbnB1dFNsb3Q6QXV0bwAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24MAFBSSU5URVJfTkFNRRAATUZDLTE5MTBXLXNlcmllcwsARFJJVkVSX05BTUUVAENVUFM6TUZDLTE5MTBXLXNlcmllcw==</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -1941,7 +1974,6 @@
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
-    <style:font-face style:name="Liberation Serif" svg:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans Arabic" svg:font-family="'Noto Sans Arabic'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Noto Sans Devanagari" svg:font-family="'Noto Sans Devanagari'" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -1956,7 +1988,7 @@
       <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" loext:tab-stop-distance="0in" style:writing-mode="page" style:font-independent-line-spacing="false">
         <style:tab-stops/>
       </style:paragraph-properties>
-      <style:text-properties style:use-window-font-color="true" loext:opacity="0%" style:font-name="Liberation Serif" fo:font-size="12pt" fo:language="en" fo:country="US" style:letter-kerning="true" style:font-name-asian="DejaVu Sans" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-family-complex="'Noto Sans'" style:font-family-generic-complex="system" style:font-pitch-complex="variable" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN"/>
+      <style:text-properties style:use-window-font-color="true" loext:opacity="0%" fo:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable" fo:font-size="12pt" fo:language="en" fo:country="US" style:letter-kerning="true" style:font-name-asian="DejaVu Sans" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-family-complex="'Noto Sans'" style:font-family-generic-complex="system" style:font-pitch-complex="variable" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN"/>
     </style:default-style>
     <style:style style:name="Default" style:family="graphic"/>
     <style:style style:name="Note" style:family="graphic" style:parent-style-name="Default">
@@ -2081,7 +2113,7 @@
     </number:date-style>
     <number:number-style style:name="N145P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N145">
       <style:text-properties fo:color="#ff0000"/>
@@ -2092,7 +2124,7 @@
     </number:number-style>
     <number:number-style style:name="N147P0" style:volatile="true">
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N147">
       <style:text-properties fo:color="#ff0000"/>
@@ -2102,40 +2134,38 @@
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N147P0"/>
     </number:number-style>
     <number:number-style style:name="N151P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N151P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N151P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>- _)</number:text>
     </number:number-style>
     <number:text-style style:name="N151">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N151P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N151P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N151P2"/>
     </number:text-style>
     <number:currency-style style:name="N155P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> _)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N155P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
@@ -2143,56 +2173,53 @@
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N155P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>- _)</number:text>
     </number:currency-style>
     <number:text-style style:name="N155">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N155P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N155P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N155P2"/>
     </number:text-style>
     <number:number-style style:name="N159P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N159P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N159P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="2" loext:max-blank-integer-digits="2"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
     </number:number-style>
     <number:text-style style:name="N159">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N159P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N159P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N159P2"/>
     </number:text-style>
     <number:currency-style style:name="N163P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> _)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N163P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
@@ -2200,7 +2227,6 @@
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N163P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
@@ -2208,9 +2234,9 @@
       <number:text> _)</number:text>
     </number:currency-style>
     <number:text-style style:name="N163">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N163P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N163P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N163P2"/>
@@ -2238,7 +2264,7 @@
     <number:currency-style style:name="N169P0" style:volatile="true">
       <number:currency-symbol/>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N169">
       <number:text>(</number:text>
@@ -2250,7 +2276,7 @@
     <number:currency-style style:name="N170P0" style:volatile="true">
       <number:currency-symbol/>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N170">
       <style:text-properties fo:color="#ff0000"/>
@@ -2263,7 +2289,7 @@
     <number:currency-style style:name="N172P0" style:volatile="true">
       <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N172">
       <number:text>(</number:text>
@@ -2275,7 +2301,7 @@
     <number:currency-style style:name="N173P0" style:volatile="true">
       <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N173">
       <style:text-properties fo:color="#ff0000"/>
@@ -2286,40 +2312,38 @@
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N173P0"/>
     </number:currency-style>
     <number:number-style style:name="N175P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
     </number:number-style>
     <number:number-style style:name="N175P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
     <number:number-style style:name="N175P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:text>- _)</number:text>
+      <number:text>- </number:text>
     </number:number-style>
     <number:text-style style:name="N175">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N175P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N175P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N175P2"/>
     </number:text-style>
     <number:currency-style style:name="N178P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N178P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
@@ -2327,28 +2351,25 @@
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N178P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
-      <number:text>- _)</number:text>
+      <number:text>- </number:text>
     </number:currency-style>
     <number:text-style style:name="N178">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N178P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N178P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N178P2"/>
     </number:text-style>
     <number:currency-style style:name="N181P0" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N181P1" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
@@ -2356,17 +2377,16 @@
       <number:text>)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N181P2" style:volatile="true">
-      <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="2" loext:max-blank-integer-digits="2"/>
-      <number:text> _)</number:text>
+      <number:text> </number:text>
     </number:currency-style>
     <number:text-style style:name="N181">
-      <number:text loext:blank-width-char="("> </number:text>
+      <number:text> </number:text>
       <number:text-content/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> </number:text>
       <style:map style:condition="value()&gt;0" style:apply-style-name="N181P0"/>
       <style:map style:condition="value()&lt;0" style:apply-style-name="N181P1"/>
       <style:map style:condition="value()=0" style:apply-style-name="N181P2"/>
@@ -2469,22 +2489,6 @@
       <style:text-properties fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="bold" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-style-complex="italic" style:font-weight-complex="bold"/>
     </style:style>
     <draw:marker draw:name="Arrowheads_20_1" draw:display-name="Arrowheads 1" svg:viewBox="0 0 20 30" svg:d="M10 0l-10 30h20z"/>
-    <loext:theme loext:name="ערכת נושא של Office 2013 - 2022">
-      <loext:theme-colors loext:name="Office 2013 - 2022">
-        <loext:color loext:name="dark1" loext:color="#000000"/>
-        <loext:color loext:name="light1" loext:color="#ffffff"/>
-        <loext:color loext:name="dark2" loext:color="#44546a"/>
-        <loext:color loext:name="light2" loext:color="#e7e6e6"/>
-        <loext:color loext:name="accent1" loext:color="#4472c4"/>
-        <loext:color loext:name="accent2" loext:color="#ed7d31"/>
-        <loext:color loext:name="accent3" loext:color="#a5a5a5"/>
-        <loext:color loext:name="accent4" loext:color="#ffc000"/>
-        <loext:color loext:name="accent5" loext:color="#5b9bd5"/>
-        <loext:color loext:name="accent6" loext:color="#70ad47"/>
-        <loext:color loext:name="hyperlink" loext:color="#0563c1"/>
-        <loext:color loext:name="followed-hyperlink" loext:color="#954f72"/>
-      </loext:theme-colors>
-    </loext:theme>
   </office:styles>
   <office:automatic-styles>
     <number:number-style style:name="N2">
@@ -2555,7 +2559,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2024-07-17">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="12:06:02.323167599">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="21:23:46.718996285">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>